<commit_message>
[feat] google calendar fix and text align
</commit_message>
<xml_diff>
--- a/마고의바다.xlsx
+++ b/마고의바다.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Polaris Office Sheet" lastEdited="4" lowestEdited="4" rupBuild="9.104.197.51428"/>
+  <fileVersion appName="Polaris Office Sheet" lastEdited="4" lowestEdited="4" rupBuild="10.105.228.52576"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="590" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -776,7 +776,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -791,7 +790,6 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -800,7 +798,6 @@
       <bottom style="thick">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -809,7 +806,6 @@
       <bottom style="thick">
         <color rgb="FFACCCEA"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -818,7 +814,6 @@
       <bottom style="medium">
         <color theme="4" tint="0.399980"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -833,7 +828,6 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -848,7 +842,6 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="double">
@@ -863,7 +856,6 @@
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -872,7 +864,6 @@
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -883,7 +874,6 @@
       <bottom style="double">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
@@ -1035,7 +1025,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1052,9 +1042,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1378,7 +1365,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
@@ -1446,7 +1433,7 @@
       <c r="A9" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1454,7 +1441,7 @@
       <c r="A10" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1462,7 +1449,7 @@
       <c r="A11" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="1" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1470,22 +1457,22 @@
       <c r="A12" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="1" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>